<commit_message>
Perubahan database dan excel
</commit_message>
<xml_diff>
--- a/Master Data F1.xlsx
+++ b/Master Data F1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>REKAPITULASI PROSENTASE KEHADIRAN DOSEN</t>
   </si>
@@ -137,6 +137,12 @@
     <t>Aljabar Linier</t>
   </si>
   <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
     <t>2020/2021</t>
   </si>
   <si>
@@ -152,6 +158,12 @@
     <t xml:space="preserve"> Bahasa Inggris untuk TIK 2</t>
   </si>
   <si>
+    <t>93,33%</t>
+  </si>
+  <si>
+    <t>6,67%</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Risna Sari, S.Kom., M.T.i</t>
   </si>
   <si>
@@ -168,6 +180,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Pemrograman Web 1</t>
+  </si>
+  <si>
+    <t>93,75%</t>
+  </si>
+  <si>
+    <t>6,25%</t>
   </si>
   <si>
     <t xml:space="preserve"> Euis Oktavianti, S.Si, M.T.i</t>
@@ -938,11 +956,11 @@
       <c r="W7" s="4">
         <v>1</v>
       </c>
-      <c r="X7" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="4">
-        <v>0</v>
+      <c r="X7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="Z7" s="4">
         <v>56</v>
@@ -960,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="AE7" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -968,13 +986,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2">
         <v>1819117681</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -1029,11 +1047,11 @@
       <c r="W8" s="4">
         <v>1</v>
       </c>
-      <c r="X8" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="4">
-        <v>0</v>
+      <c r="X8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="Z8" s="4">
         <v>64</v>
@@ -1051,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="AE8" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -1059,13 +1077,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2">
         <v>1819117682</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1118,11 +1136,11 @@
       <c r="W9" s="4">
         <v>1</v>
       </c>
-      <c r="X9" s="4">
-        <v>0.9333</v>
-      </c>
-      <c r="Y9" s="4">
-        <v>0.0667</v>
+      <c r="X9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="Z9" s="4">
         <v>42</v>
@@ -1140,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -1148,13 +1166,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2">
         <v>1819117683</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1211,11 +1229,11 @@
       <c r="W10" s="4">
         <v>1</v>
       </c>
-      <c r="X10" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="4">
-        <v>0</v>
+      <c r="X10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="Z10" s="4">
         <v>80</v>
@@ -1233,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="AE10" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -1241,13 +1259,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2">
         <v>1819117684</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4">
@@ -1265,7 +1283,9 @@
       <c r="J11" s="4">
         <v>1</v>
       </c>
-      <c r="K11" s="4"/>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
       <c r="L11" s="4">
         <v>1</v>
       </c>
@@ -1298,11 +1318,11 @@
       <c r="W11" s="4">
         <v>1</v>
       </c>
-      <c r="X11" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="4">
-        <v>0</v>
+      <c r="X11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="Z11" s="4">
         <v>84</v>
@@ -1320,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="AE11" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -1328,13 +1348,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2">
         <v>1819117685</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -1389,11 +1409,11 @@
       <c r="W12" s="4">
         <v>1</v>
       </c>
-      <c r="X12" s="4">
-        <v>0.9375</v>
-      </c>
-      <c r="Y12" s="4">
-        <v>0.0625</v>
+      <c r="X12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="Z12" s="4">
         <v>77</v>
@@ -1411,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="AE12" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -1419,13 +1439,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2">
         <v>1819117686</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E13" s="4">
         <v>1</v>
@@ -1480,11 +1500,11 @@
       <c r="W13" s="4">
         <v>1</v>
       </c>
-      <c r="X13" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="4">
-        <v>0</v>
+      <c r="X13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="Z13" s="4">
         <v>45</v>
@@ -1502,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="AE13" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -1510,13 +1530,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2">
         <v>1819117687</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4">
@@ -1569,11 +1589,11 @@
       <c r="W14" s="4">
         <v>1</v>
       </c>
-      <c r="X14" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="4">
-        <v>0</v>
+      <c r="X14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="Z14" s="4">
         <v>102</v>
@@ -1591,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="AE14" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>